<commit_message>
docs: chỉnh xong file word và uml
</commit_message>
<xml_diff>
--- a/docs/Test Cases.xlsx
+++ b/docs/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuth\Desktop\lVTN_Project\lvtn_indieGameForum\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B753735-97E3-4015-A218-427286208AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6745CFC4-7F66-4EC2-AE9A-337B9BDA987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Build 1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="125">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -108,9 +108,6 @@
     <t>TC_DANGKY_02</t>
   </si>
   <si>
-    <t>Kiểm thử người dùng nhập username không hợp lệ (rỗng)</t>
-  </si>
-  <si>
     <t>1. Người dùng nhập địa chỉ Email đúng định dạng</t>
   </si>
   <si>
@@ -124,6 +121,285 @@
   </si>
   <si>
     <t>Hiển thị thông báo "Vui lòng nhập Tên đăng nhập"</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng nhập một trường bất kỳ không hợp lệ (rỗng)</t>
+  </si>
+  <si>
+    <t>Kiểm thử khi người dùng đăng ký với username hoặc Email đã được sử dụng</t>
+  </si>
+  <si>
+    <t>2. Người dùng nhập địa chỉ Email đúng định dạng và đã được sử dụng bới tài khoản khác</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo "Email đã được sử dụng"</t>
+  </si>
+  <si>
+    <t>username: thaipham123</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>TC_DANGKY_03</t>
+  </si>
+  <si>
+    <t>TS_SGDGI_02</t>
+  </si>
+  <si>
+    <t>TC_DANGNHAP_01</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng tìm kiếm dự án  và lọc dự án theo giá tăng dần</t>
+  </si>
+  <si>
+    <t>1. Nhập từ khoá tìm kiếm và nhấn Enter</t>
+  </si>
+  <si>
+    <t>2. Chọn bộ lọc theo giá</t>
+  </si>
+  <si>
+    <t>3. Chọn thứ tự tăng dần</t>
+  </si>
+  <si>
+    <t>4. Bấm nút xem</t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách dự án trùng khớp</t>
+  </si>
+  <si>
+    <t>LAZR</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>TC_DANGNHAP_02</t>
+  </si>
+  <si>
+    <t>TC_TIMKIEM_01</t>
+  </si>
+  <si>
+    <t>TS_SGDGI_03</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng đăng nhập với thông tin tài khoản chính xác</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng đăng nhập với thông tin tài khoản sai</t>
+  </si>
+  <si>
+    <t>1. Nhập tên tài khoản đã đăng ký</t>
+  </si>
+  <si>
+    <t>2. Nhập mật khẩu đúng</t>
+  </si>
+  <si>
+    <t>3. Bấm nút đăng nhập</t>
+  </si>
+  <si>
+    <t>2. Nhập mật khẩu sai</t>
+  </si>
+  <si>
+    <t>Đăng nhập thành công! Điều hướng đến trang chủ</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo "Sai thông tin đăng nhập! Vui lòng thử lại"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password: Xtera123 </t>
+  </si>
+  <si>
+    <t>password: Xtera123d3</t>
+  </si>
+  <si>
+    <t>TC_TIMKIEM_02</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng tìm kiếm dự án với từ khoá không tồn tại</t>
+  </si>
+  <si>
+    <t>Hiển thị text "Không có dự án nào trùng khớp"</t>
+  </si>
+  <si>
+    <t>Axis</t>
+  </si>
+  <si>
+    <t>TS_SGDGI_04</t>
+  </si>
+  <si>
+    <t>TC_DANGDUAN_02</t>
+  </si>
+  <si>
+    <t>TC_DANGDUAN_01</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng đăng dự án với các thông tin hợp lệ, có hình ảnh và tệp dự án</t>
+  </si>
+  <si>
+    <t>1. Nhập các thông tin mô tả dự án</t>
+  </si>
+  <si>
+    <t>2. Chọn ảnh</t>
+  </si>
+  <si>
+    <t>3. Chọn tệp dự án</t>
+  </si>
+  <si>
+    <t>4. Xác nhận đăng dự án mới</t>
+  </si>
+  <si>
+    <t>Thông báo quá trình tải lên ảnh và tệp dự án. Sau đó điều hướng đến trang xem trước dự án</t>
+  </si>
+  <si>
+    <t>Tên dự án: Axis, loại: trò chơi, thể loại: hành động, 2d, phiêu lưu</t>
+  </si>
+  <si>
+    <t>Mô tả ngắn: mô tả ngắn</t>
+  </si>
+  <si>
+    <t>Mô tả chi tiết: Mô tả chi tiết</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng đăng dự án với các thông tin hợp lệ, không có ảnh, có tệp dự án</t>
+  </si>
+  <si>
+    <t>3. Xác nhận đăng dự án mới</t>
+  </si>
+  <si>
+    <t>Thông báo quá trình tải lên tệp dự án. Sau đó điều hướng đến trang xem trước dự án</t>
+  </si>
+  <si>
+    <t>Tệp dự án cho: windows, android, ios, Hiển thị: riêng tư</t>
+  </si>
+  <si>
+    <t>Chọn ảnh bìa và ảnh màn hình</t>
+  </si>
+  <si>
+    <t>TC_DANGDUAN_03</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng đăng dự án với các thông tin hợp lệ, không có ảnh, và không có tệp dự án</t>
+  </si>
+  <si>
+    <t>2. Chọn tệp dự án</t>
+  </si>
+  <si>
+    <t>2. Xác nhận đăng dự án mới</t>
+  </si>
+  <si>
+    <t>Thông báo quá trình lên thông tin dự án. Sau đó điều hướng đến trang xem trước dự án</t>
+  </si>
+  <si>
+    <t>TC_DANGDUAN_04</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng đăng dự án với thông tin không có tên dự án</t>
+  </si>
+  <si>
+    <t>1. Nhập các thông tin mô tả dự án, bỏ trống tên dự án</t>
+  </si>
+  <si>
+    <t>Thông báo quá trình lên không thành công</t>
+  </si>
+  <si>
+    <t>Tên dự án: "", loại: trò chơi, thể loại: hành động, 2d, phiêu lưu</t>
+  </si>
+  <si>
+    <t>TS_SGDGI_05</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng chỉnh sửa dự án với thông tin hợp lệ</t>
+  </si>
+  <si>
+    <t>1. Điều chỉnh thông tin mô tả dự án cần chỉnh sửa</t>
+  </si>
+  <si>
+    <t>2. Xác nhận lưu chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thành công. Sau đó điều hướng đến trang xem trước dự án</t>
+  </si>
+  <si>
+    <t>Tên dự án điều chỉnh: Axxis 01</t>
+  </si>
+  <si>
+    <t>TC_CHINHSUADUAN_01</t>
+  </si>
+  <si>
+    <t>Kiểm thử người dùng chỉnh sửa dự án với tên dự án bỏ trống</t>
+  </si>
+  <si>
+    <t>1. Điều chỉnh thông tin mô tả dự án cần chỉnh sửa. Xoá hết tên dự án cũ</t>
+  </si>
+  <si>
+    <t>Thông báo tên dự án không được để trống</t>
+  </si>
+  <si>
+    <t>Tên dự án điều chỉnh: " "</t>
+  </si>
+  <si>
+    <t>TC_CHINHSUADUAN_02</t>
+  </si>
+  <si>
+    <t>TC_CAPNHATANH_02</t>
+  </si>
+  <si>
+    <t>TS_SGDGI_06</t>
+  </si>
+  <si>
+    <t>Kiểm thử khi người dùng cập nhật hình ảnh bìa nhỏ cho dự án</t>
+  </si>
+  <si>
+    <t>1. Ấn nút cập nhật hình ảnh trong giao diện xem trước dự án</t>
+  </si>
+  <si>
+    <t>2. Chọn ảnh bìa nhỏ</t>
+  </si>
+  <si>
+    <t>3. Nhấn cập nhật</t>
+  </si>
+  <si>
+    <t>Hiển thị hiệu ứng cập nhât và reload lại trang</t>
+  </si>
+  <si>
+    <t>Chọn ảnh bìa nhỏ</t>
+  </si>
+  <si>
+    <t>TC_CAPNHATANH_01</t>
+  </si>
+  <si>
+    <t>Kiểm thử khi người dùng cập nhật hình ảnh bìa lớn cho dự án</t>
+  </si>
+  <si>
+    <t>2. Chọn ảnh bìa lớn</t>
+  </si>
+  <si>
+    <t>Chọn ảnh bìa lớn</t>
+  </si>
+  <si>
+    <t>TC_CAPNHATANH_03</t>
+  </si>
+  <si>
+    <t>Kiểm thử khi người dùng cập nhật hình ảnh màn hình cho dự án</t>
+  </si>
+  <si>
+    <t>2. Chọn nhiều ảnh màn hình</t>
+  </si>
+  <si>
+    <t>Chọn nhiều ảnh màn hình</t>
+  </si>
+  <si>
+    <t>TC_CAPNHATANH_04</t>
+  </si>
+  <si>
+    <t>Kiểm thử khi người dùng cập nhật hình ảnh màn hình, ảnh bìa lớn và ảnh bìa nhỏ cho dự án</t>
+  </si>
+  <si>
+    <t>2. Chọn ảnh bìa lớn, chọn ảnh bìa nhỏ, chọn nhiều ảnh màn hình</t>
+  </si>
+  <si>
+    <t>Chọn các hình ảnh cần cập nhật</t>
   </si>
 </sst>
 </file>
@@ -235,27 +511,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -264,7 +534,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,19 +775,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108:J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.8984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="47" style="1" customWidth="1"/>
+    <col min="3" max="3" width="86.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.8984375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="83.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.3984375" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.19921875" style="1" customWidth="1"/>
     <col min="10" max="10" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
@@ -506,299 +796,1573 @@
     <col min="27" max="16384" width="12.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="6" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="9"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="1" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="9"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="1" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="9"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="1" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J20" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="7"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="7"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="7"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="7"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="2"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+    </row>
+    <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+    </row>
+    <row r="73" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+    </row>
+    <row r="81" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+    </row>
+    <row r="84" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+    </row>
+    <row r="85" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+    </row>
+    <row r="86" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+    </row>
+    <row r="87" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+    </row>
+    <row r="91" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+    </row>
+    <row r="92" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+    </row>
+    <row r="93" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+    </row>
+    <row r="94" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H95" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+    </row>
+    <row r="97" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+    </row>
+    <row r="98" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+    </row>
+    <row r="99" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+    </row>
+    <row r="100" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+    </row>
+    <row r="101" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="10"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="4"/>
+    </row>
+    <row r="104" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="10"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
+    </row>
+    <row r="105" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="10"/>
+      <c r="C105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
+    </row>
+    <row r="106" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
+    </row>
+    <row r="107" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J108" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="4"/>
+    </row>
+    <row r="110" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="10"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="4"/>
+    </row>
+    <row r="111" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4"/>
+      <c r="B111" s="10"/>
+      <c r="C111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+    </row>
+    <row r="112" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+    </row>
     <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1688,7 +3252,127 @@
     <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="132">
+    <mergeCell ref="H102:H106"/>
+    <mergeCell ref="I102:I106"/>
+    <mergeCell ref="J102:J106"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="C108:C112"/>
+    <mergeCell ref="E108:E112"/>
+    <mergeCell ref="F108:F112"/>
+    <mergeCell ref="H108:H112"/>
+    <mergeCell ref="I108:I112"/>
+    <mergeCell ref="J108:J112"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="C102:C106"/>
+    <mergeCell ref="E102:E106"/>
+    <mergeCell ref="F102:F106"/>
+    <mergeCell ref="H89:H93"/>
+    <mergeCell ref="I89:I93"/>
+    <mergeCell ref="J89:J93"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="C96:C100"/>
+    <mergeCell ref="E96:E100"/>
+    <mergeCell ref="F96:F100"/>
+    <mergeCell ref="H95:H99"/>
+    <mergeCell ref="I95:I99"/>
+    <mergeCell ref="J95:J99"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="E89:E93"/>
+    <mergeCell ref="F89:F93"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="F82:F86"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="I76:I80"/>
+    <mergeCell ref="J76:J80"/>
+    <mergeCell ref="H82:H86"/>
+    <mergeCell ref="I82:I86"/>
+    <mergeCell ref="J82:J86"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="H62:H67"/>
+    <mergeCell ref="I62:I67"/>
+    <mergeCell ref="J62:J67"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="E69:E74"/>
+    <mergeCell ref="F69:F74"/>
+    <mergeCell ref="H69:H74"/>
+    <mergeCell ref="I69:I74"/>
+    <mergeCell ref="J69:J74"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="E62:E67"/>
+    <mergeCell ref="F62:F67"/>
+    <mergeCell ref="H48:H53"/>
+    <mergeCell ref="I48:I53"/>
+    <mergeCell ref="J48:J53"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="E55:E60"/>
+    <mergeCell ref="F55:F60"/>
+    <mergeCell ref="H55:H60"/>
+    <mergeCell ref="I55:I60"/>
+    <mergeCell ref="J55:J60"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="E48:E53"/>
+    <mergeCell ref="F48:F53"/>
+    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="F41:F46"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="H34:H38"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="B20:B25"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>

</xml_diff>

<commit_message>
feat & docs: fix lỗi ppt, edit bài viết, fix demo trước báo cáo
</commit_message>
<xml_diff>
--- a/docs/Test Cases.xlsx
+++ b/docs/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuth\Desktop\lVTN_Project\lvtn_indieGameForum\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6745CFC4-7F66-4EC2-AE9A-337B9BDA987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4DC6C0-B951-4E0D-9151-684497ADF0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="126">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>Chọn các hình ảnh cần cập nhật</t>
+  </si>
+  <si>
+    <t>TC_CAPNHATDUAN_01</t>
   </si>
 </sst>
 </file>
@@ -522,26 +525,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,6 +541,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108:J112"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -797,47 +800,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -852,20 +855,20 @@
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
@@ -874,14 +877,14 @@
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="4"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
@@ -890,14 +893,14 @@
       <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="4"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
@@ -906,14 +909,14 @@
       <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="4"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
@@ -929,13 +932,13 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -950,20 +953,20 @@
       <c r="G8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
@@ -972,14 +975,14 @@
       <c r="G9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="4"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
@@ -988,36 +991,36 @@
       <c r="G10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="4"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="4"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1026,78 +1029,78 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="10" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="4"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="4"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="4"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
@@ -1106,13 +1109,13 @@
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1121,77 +1124,77 @@
       <c r="E20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="4"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="4"/>
+      <c r="F22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="4"/>
+      <c r="F23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="4"/>
+      <c r="F24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1200,187 +1203,187 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="4"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="4"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="4"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="4"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="I32" s="8"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="2"/>
-      <c r="I33" s="8"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="14" t="s">
         <v>46</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="7"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="4"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="14"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="7"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="4"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="14"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="7"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="4"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="14"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="7"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="4"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="14"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="2"/>
       <c r="F39" s="3"/>
     </row>
@@ -1388,657 +1391,657 @@
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="10" t="s">
         <v>64</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="I41" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="4"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="10"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="4"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="10"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="4"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="10"/>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="4"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="10"/>
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I48" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="4"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
     </row>
     <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
       <c r="G50" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
     </row>
     <row r="51" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="4"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
       <c r="G51" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
     </row>
     <row r="52" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="4"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
       <c r="G52" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
     </row>
     <row r="53" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
     </row>
     <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="10" t="s">
         <v>78</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H55" s="4" t="s">
+      <c r="H55" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I55" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="J55" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="4"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="10"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
       <c r="G56" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
     </row>
     <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="4"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="10"/>
       <c r="D57" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
       <c r="G57" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="4"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
       <c r="G58" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
     </row>
     <row r="59" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="4"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
     </row>
     <row r="60" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="4"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="10"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
     </row>
     <row r="61" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="10" t="s">
         <v>84</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="10" t="s">
         <v>87</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="H62" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I62" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J62" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="4"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="10"/>
       <c r="D63" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
       <c r="G63" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
     </row>
     <row r="64" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="4"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
       <c r="G64" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
     </row>
     <row r="65" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="4"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="10"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
     </row>
     <row r="66" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="4"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="10"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
     </row>
     <row r="67" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="4"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
     </row>
     <row r="68" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="10" t="s">
         <v>89</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="F69" s="10" t="s">
         <v>91</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H69" s="4" t="s">
+      <c r="H69" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I69" s="4" t="s">
+      <c r="I69" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J69" s="4" t="s">
+      <c r="J69" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="4"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="10"/>
       <c r="D70" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
       <c r="G70" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
     </row>
     <row r="71" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="4"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="10"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
       <c r="G71" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
     </row>
     <row r="72" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="4"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="10"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
     </row>
     <row r="73" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="4"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="10"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
     </row>
     <row r="74" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="4"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="10"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
     </row>
     <row r="75" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="10" t="s">
         <v>94</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="F76" s="4" t="s">
+      <c r="F76" s="10" t="s">
         <v>97</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H76" s="4" t="s">
+      <c r="H76" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I76" s="4" t="s">
+      <c r="I76" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J76" s="4" t="s">
+      <c r="J76" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="4"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="10"/>
       <c r="D77" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
     </row>
     <row r="78" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="4"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="10"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
     </row>
     <row r="79" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="4"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="10"/>
       <c r="D79" s="2"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
     </row>
     <row r="80" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="4"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="10"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10"/>
     </row>
     <row r="81" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="10" t="s">
         <v>100</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="F82" s="10" t="s">
         <v>102</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H82" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="I82" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="J82" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="4"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="10"/>
       <c r="D83" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
     </row>
     <row r="84" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="4"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="10"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
     </row>
     <row r="85" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="4"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="10"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="10"/>
     </row>
     <row r="86" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="4"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="10"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="10"/>
     </row>
     <row r="87" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D87" s="2"/>
@@ -2047,338 +2050,350 @@
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E89" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="F89" s="10" t="s">
         <v>111</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="H89" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="I89" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J89" s="4" t="s">
+      <c r="J89" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="4"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="10"/>
       <c r="D90" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
     </row>
     <row r="91" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="4"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="10"/>
       <c r="D91" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
     </row>
     <row r="92" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
     </row>
     <row r="93" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
     </row>
     <row r="94" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H95" s="4" t="s">
+      <c r="H95" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I95" s="4" t="s">
+      <c r="I95" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J95" s="4" t="s">
+      <c r="J95" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E96" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="F96" s="10" t="s">
         <v>111</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="4"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10"/>
     </row>
     <row r="97" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="4"/>
+      <c r="A97" s="10"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="10"/>
       <c r="D97" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
     </row>
     <row r="98" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="4"/>
+      <c r="A98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="10"/>
       <c r="D98" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="4"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="10"/>
     </row>
     <row r="99" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="10"/>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
+      <c r="A99" s="10"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10"/>
     </row>
     <row r="100" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
     </row>
     <row r="101" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="102" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B102" s="10" t="s">
+      <c r="B102" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="10" t="s">
         <v>118</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E102" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F102" s="4" t="s">
+      <c r="F102" s="10" t="s">
         <v>111</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H102" s="4" t="s">
+      <c r="H102" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I102" s="4" t="s">
+      <c r="I102" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J102" s="4" t="s">
+      <c r="J102" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="10"/>
-      <c r="C103" s="4"/>
+      <c r="A103" s="10"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="10"/>
       <c r="D103" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="10"/>
     </row>
     <row r="104" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="4"/>
+      <c r="A104" s="10"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="10"/>
       <c r="D104" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="J104" s="4"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="J104" s="10"/>
     </row>
     <row r="105" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
-      <c r="J105" s="4"/>
+      <c r="A105" s="10"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
     </row>
     <row r="106" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
-      <c r="J106" s="4"/>
+      <c r="A106" s="10"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
     </row>
     <row r="107" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="108" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B108" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="10" t="s">
         <v>122</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E108" s="4" t="s">
+      <c r="E108" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F108" s="4" t="s">
+      <c r="F108" s="10" t="s">
         <v>111</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H108" s="4" t="s">
+      <c r="H108" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="I108" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J108" s="4" t="s">
+      <c r="J108" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="4"/>
+      <c r="A109" s="10"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="10"/>
       <c r="D109" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
-      <c r="J109" s="4"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="J109" s="10"/>
     </row>
     <row r="110" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="4"/>
+      <c r="A110" s="10"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="10"/>
       <c r="D110" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+      <c r="J110" s="10"/>
     </row>
     <row r="111" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="4"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="4"/>
-      <c r="J111" s="4"/>
+      <c r="A111" s="10"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="J111" s="10"/>
     </row>
     <row r="112" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="4"/>
-    </row>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A112" s="10"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="J112" s="10"/>
+    </row>
+    <row r="113" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="10"/>
+    </row>
+    <row r="117" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="10"/>
+    </row>
+    <row r="118" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="10"/>
+    </row>
+    <row r="119" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="10"/>
+    </row>
+    <row r="120" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3252,87 +3267,43 @@
     <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="132">
-    <mergeCell ref="H102:H106"/>
-    <mergeCell ref="I102:I106"/>
-    <mergeCell ref="J102:J106"/>
-    <mergeCell ref="A108:A112"/>
-    <mergeCell ref="B108:B112"/>
-    <mergeCell ref="C108:C112"/>
-    <mergeCell ref="E108:E112"/>
-    <mergeCell ref="F108:F112"/>
-    <mergeCell ref="H108:H112"/>
-    <mergeCell ref="I108:I112"/>
-    <mergeCell ref="J108:J112"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="B102:B106"/>
-    <mergeCell ref="C102:C106"/>
-    <mergeCell ref="E102:E106"/>
-    <mergeCell ref="F102:F106"/>
-    <mergeCell ref="H89:H93"/>
-    <mergeCell ref="I89:I93"/>
-    <mergeCell ref="J89:J93"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="C96:C100"/>
-    <mergeCell ref="E96:E100"/>
-    <mergeCell ref="F96:F100"/>
-    <mergeCell ref="H95:H99"/>
-    <mergeCell ref="I95:I99"/>
-    <mergeCell ref="J95:J99"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="C89:C93"/>
-    <mergeCell ref="E89:E93"/>
-    <mergeCell ref="F89:F93"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="F82:F86"/>
-    <mergeCell ref="H76:H80"/>
-    <mergeCell ref="I76:I80"/>
-    <mergeCell ref="J76:J80"/>
-    <mergeCell ref="H82:H86"/>
-    <mergeCell ref="I82:I86"/>
-    <mergeCell ref="J82:J86"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="E76:E80"/>
-    <mergeCell ref="F76:F80"/>
-    <mergeCell ref="H62:H67"/>
-    <mergeCell ref="I62:I67"/>
-    <mergeCell ref="J62:J67"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="B69:B74"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="E69:E74"/>
-    <mergeCell ref="F69:F74"/>
-    <mergeCell ref="H69:H74"/>
-    <mergeCell ref="I69:I74"/>
-    <mergeCell ref="J69:J74"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="E62:E67"/>
-    <mergeCell ref="F62:F67"/>
-    <mergeCell ref="H48:H53"/>
-    <mergeCell ref="I48:I53"/>
-    <mergeCell ref="J48:J53"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="C55:C60"/>
-    <mergeCell ref="E55:E60"/>
-    <mergeCell ref="F55:F60"/>
-    <mergeCell ref="H55:H60"/>
-    <mergeCell ref="I55:I60"/>
-    <mergeCell ref="J55:J60"/>
-    <mergeCell ref="A48:A53"/>
-    <mergeCell ref="B48:B53"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="E48:E53"/>
-    <mergeCell ref="F48:F53"/>
+  <mergeCells count="133">
+    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
     <mergeCell ref="J27:J31"/>
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="B41:B46"/>
@@ -3350,41 +3321,86 @@
     <mergeCell ref="I34:I38"/>
     <mergeCell ref="J34:J38"/>
     <mergeCell ref="F27:F32"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="J20:J24"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="I14:I17"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="H48:H53"/>
+    <mergeCell ref="I48:I53"/>
+    <mergeCell ref="J48:J53"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="E55:E60"/>
+    <mergeCell ref="F55:F60"/>
+    <mergeCell ref="H55:H60"/>
+    <mergeCell ref="I55:I60"/>
+    <mergeCell ref="J55:J60"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="E48:E53"/>
+    <mergeCell ref="F48:F53"/>
+    <mergeCell ref="H62:H67"/>
+    <mergeCell ref="I62:I67"/>
+    <mergeCell ref="J62:J67"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="E69:E74"/>
+    <mergeCell ref="F69:F74"/>
+    <mergeCell ref="H69:H74"/>
+    <mergeCell ref="I69:I74"/>
+    <mergeCell ref="J69:J74"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="E62:E67"/>
+    <mergeCell ref="F62:F67"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="F82:F86"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="I76:I80"/>
+    <mergeCell ref="J76:J80"/>
+    <mergeCell ref="H82:H86"/>
+    <mergeCell ref="I82:I86"/>
+    <mergeCell ref="J82:J86"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="H89:H93"/>
+    <mergeCell ref="I89:I93"/>
+    <mergeCell ref="J89:J93"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="C96:C100"/>
+    <mergeCell ref="E96:E100"/>
+    <mergeCell ref="F96:F100"/>
+    <mergeCell ref="H95:H99"/>
+    <mergeCell ref="I95:I99"/>
+    <mergeCell ref="J95:J99"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="E89:E93"/>
+    <mergeCell ref="F89:F93"/>
+    <mergeCell ref="H102:H106"/>
+    <mergeCell ref="I102:I106"/>
+    <mergeCell ref="J102:J106"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="C108:C112"/>
+    <mergeCell ref="E108:E112"/>
+    <mergeCell ref="F108:F112"/>
+    <mergeCell ref="H108:H112"/>
+    <mergeCell ref="I108:I112"/>
+    <mergeCell ref="J108:J112"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="C102:C106"/>
+    <mergeCell ref="E102:E106"/>
+    <mergeCell ref="F102:F106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: Share thư mục phiên bản mới cho người mua
</commit_message>
<xml_diff>
--- a/docs/Test Cases.xlsx
+++ b/docs/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuth\Desktop\lVTN_Project\lvtn_indieGameForum\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D286734-0201-406F-B293-E5799919C3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4985FEC9-F19C-4383-ABDF-6CECFA69A853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,8 +999,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1011,8 +1011,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,7 +1231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A270" sqref="A270:A275"/>
     </sheetView>
   </sheetViews>
@@ -1853,7 +1853,7 @@
       <c r="C41" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="20" t="s">
         <v>42</v>
       </c>
       <c r="E41" s="13" t="s">
@@ -1879,7 +1879,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="H42" s="13"/>
@@ -4041,10 +4041,10 @@
       <c r="D207" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E207" s="20" t="s">
+      <c r="E207" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="F207" s="20" t="s">
+      <c r="F207" s="16" t="s">
         <v>214</v>
       </c>
       <c r="G207" s="1" t="s">
@@ -4067,8 +4067,8 @@
       <c r="D208" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E208" s="20"/>
-      <c r="F208" s="20"/>
+      <c r="E208" s="16"/>
+      <c r="F208" s="16"/>
       <c r="G208" s="1" t="s">
         <v>216</v>
       </c>
@@ -4083,8 +4083,8 @@
       <c r="D209" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E209" s="20"/>
-      <c r="F209" s="20"/>
+      <c r="E209" s="16"/>
+      <c r="F209" s="16"/>
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
       <c r="J209" s="13"/>
@@ -4096,8 +4096,8 @@
       <c r="D210" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E210" s="20"/>
-      <c r="F210" s="20"/>
+      <c r="E210" s="16"/>
+      <c r="F210" s="16"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
       <c r="J210" s="13"/>
@@ -4109,8 +4109,8 @@
       <c r="D211" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E211" s="20"/>
-      <c r="F211" s="20"/>
+      <c r="E211" s="16"/>
+      <c r="F211" s="16"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
       <c r="J211" s="13"/>
@@ -4119,8 +4119,8 @@
       <c r="A212" s="13"/>
       <c r="B212" s="14"/>
       <c r="C212" s="15"/>
-      <c r="E212" s="20"/>
-      <c r="F212" s="20"/>
+      <c r="E212" s="16"/>
+      <c r="F212" s="16"/>
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
       <c r="J212" s="13"/>
@@ -4139,10 +4139,10 @@
       <c r="D214" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E214" s="20" t="s">
+      <c r="E214" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="F214" s="20" t="s">
+      <c r="F214" s="16" t="s">
         <v>214</v>
       </c>
       <c r="G214" s="1" t="s">
@@ -4165,8 +4165,8 @@
       <c r="D215" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E215" s="20"/>
-      <c r="F215" s="20"/>
+      <c r="E215" s="16"/>
+      <c r="F215" s="16"/>
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
       <c r="J215" s="13"/>
@@ -4178,8 +4178,8 @@
       <c r="D216" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E216" s="20"/>
-      <c r="F216" s="20"/>
+      <c r="E216" s="16"/>
+      <c r="F216" s="16"/>
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
       <c r="J216" s="13"/>
@@ -4191,8 +4191,8 @@
       <c r="D217" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E217" s="20"/>
-      <c r="F217" s="20"/>
+      <c r="E217" s="16"/>
+      <c r="F217" s="16"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
       <c r="J217" s="13"/>
@@ -4204,8 +4204,8 @@
       <c r="D218" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E218" s="20"/>
-      <c r="F218" s="20"/>
+      <c r="E218" s="16"/>
+      <c r="F218" s="16"/>
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
       <c r="J218" s="13"/>
@@ -4214,8 +4214,8 @@
       <c r="A219" s="13"/>
       <c r="B219" s="14"/>
       <c r="C219" s="15"/>
-      <c r="E219" s="20"/>
-      <c r="F219" s="20"/>
+      <c r="E219" s="16"/>
+      <c r="F219" s="16"/>
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
       <c r="J219" s="13"/>
@@ -4234,10 +4234,10 @@
       <c r="D221" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E221" s="20" t="s">
+      <c r="E221" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F221" s="20" t="s">
+      <c r="F221" s="16" t="s">
         <v>226</v>
       </c>
       <c r="H221" s="13" t="s">
@@ -4257,8 +4257,8 @@
       <c r="D222" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E222" s="20"/>
-      <c r="F222" s="20"/>
+      <c r="E222" s="16"/>
+      <c r="F222" s="16"/>
       <c r="H222" s="13"/>
       <c r="I222" s="13"/>
       <c r="J222" s="13"/>
@@ -4267,8 +4267,8 @@
       <c r="A223" s="13"/>
       <c r="B223" s="14"/>
       <c r="C223" s="15"/>
-      <c r="E223" s="20"/>
-      <c r="F223" s="20"/>
+      <c r="E223" s="16"/>
+      <c r="F223" s="16"/>
       <c r="H223" s="13"/>
       <c r="I223" s="13"/>
       <c r="J223" s="13"/>
@@ -4277,8 +4277,8 @@
       <c r="A224" s="13"/>
       <c r="B224" s="14"/>
       <c r="C224" s="15"/>
-      <c r="E224" s="20"/>
-      <c r="F224" s="20"/>
+      <c r="E224" s="16"/>
+      <c r="F224" s="16"/>
       <c r="H224" s="13"/>
       <c r="I224" s="13"/>
       <c r="J224" s="13"/>
@@ -4287,8 +4287,8 @@
       <c r="A225" s="13"/>
       <c r="B225" s="14"/>
       <c r="C225" s="15"/>
-      <c r="E225" s="20"/>
-      <c r="F225" s="20"/>
+      <c r="E225" s="16"/>
+      <c r="F225" s="16"/>
       <c r="H225" s="13"/>
       <c r="I225" s="13"/>
       <c r="J225" s="13"/>
@@ -4297,8 +4297,8 @@
       <c r="A226" s="13"/>
       <c r="B226" s="14"/>
       <c r="C226" s="15"/>
-      <c r="E226" s="20"/>
-      <c r="F226" s="20"/>
+      <c r="E226" s="16"/>
+      <c r="F226" s="16"/>
       <c r="H226" s="13"/>
       <c r="I226" s="13"/>
       <c r="J226" s="13"/>
@@ -5645,38 +5645,266 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="314">
-    <mergeCell ref="H263:H268"/>
-    <mergeCell ref="I263:I268"/>
-    <mergeCell ref="J263:J268"/>
-    <mergeCell ref="H270:H275"/>
-    <mergeCell ref="I270:I275"/>
-    <mergeCell ref="J270:J275"/>
-    <mergeCell ref="A263:A268"/>
-    <mergeCell ref="B263:B268"/>
-    <mergeCell ref="C263:C268"/>
-    <mergeCell ref="A270:A275"/>
-    <mergeCell ref="B270:B275"/>
-    <mergeCell ref="C270:C275"/>
-    <mergeCell ref="E263:E267"/>
-    <mergeCell ref="E270:E274"/>
-    <mergeCell ref="F270:F274"/>
-    <mergeCell ref="F263:F267"/>
-    <mergeCell ref="B249:B254"/>
-    <mergeCell ref="A249:A254"/>
-    <mergeCell ref="C249:C254"/>
-    <mergeCell ref="E249:E254"/>
-    <mergeCell ref="F249:F254"/>
-    <mergeCell ref="H249:H254"/>
-    <mergeCell ref="I249:I254"/>
-    <mergeCell ref="J249:J254"/>
-    <mergeCell ref="A256:A261"/>
-    <mergeCell ref="B256:B261"/>
-    <mergeCell ref="C256:C261"/>
-    <mergeCell ref="E256:E261"/>
-    <mergeCell ref="F256:F261"/>
-    <mergeCell ref="H256:H261"/>
-    <mergeCell ref="I256:I261"/>
-    <mergeCell ref="J256:J261"/>
+    <mergeCell ref="H157:H162"/>
+    <mergeCell ref="I157:I162"/>
+    <mergeCell ref="J157:J162"/>
+    <mergeCell ref="H164:H169"/>
+    <mergeCell ref="I164:I169"/>
+    <mergeCell ref="J164:J169"/>
+    <mergeCell ref="E164:E168"/>
+    <mergeCell ref="F164:F168"/>
+    <mergeCell ref="A157:A162"/>
+    <mergeCell ref="B157:B162"/>
+    <mergeCell ref="C157:C162"/>
+    <mergeCell ref="C164:C169"/>
+    <mergeCell ref="E157:E161"/>
+    <mergeCell ref="F157:F161"/>
+    <mergeCell ref="B164:B169"/>
+    <mergeCell ref="B171:B176"/>
+    <mergeCell ref="A164:A169"/>
+    <mergeCell ref="A171:A176"/>
+    <mergeCell ref="A143:A148"/>
+    <mergeCell ref="B143:B148"/>
+    <mergeCell ref="C143:C148"/>
+    <mergeCell ref="E143:E148"/>
+    <mergeCell ref="F143:F148"/>
+    <mergeCell ref="E171:E175"/>
+    <mergeCell ref="F171:F175"/>
+    <mergeCell ref="H143:H148"/>
+    <mergeCell ref="I143:I148"/>
+    <mergeCell ref="J143:J148"/>
+    <mergeCell ref="A150:A155"/>
+    <mergeCell ref="B150:B155"/>
+    <mergeCell ref="C150:C155"/>
+    <mergeCell ref="E150:E154"/>
+    <mergeCell ref="F150:F154"/>
+    <mergeCell ref="H150:H155"/>
+    <mergeCell ref="I150:I155"/>
+    <mergeCell ref="J150:J155"/>
+    <mergeCell ref="J129:J134"/>
+    <mergeCell ref="A136:A141"/>
+    <mergeCell ref="B136:B141"/>
+    <mergeCell ref="C136:C141"/>
+    <mergeCell ref="E136:E141"/>
+    <mergeCell ref="F136:F141"/>
+    <mergeCell ref="H136:H141"/>
+    <mergeCell ref="I136:I141"/>
+    <mergeCell ref="J136:J141"/>
+    <mergeCell ref="A129:A134"/>
+    <mergeCell ref="B129:B134"/>
+    <mergeCell ref="C129:C134"/>
+    <mergeCell ref="E129:E134"/>
+    <mergeCell ref="F129:F134"/>
+    <mergeCell ref="H129:H134"/>
+    <mergeCell ref="I129:I134"/>
+    <mergeCell ref="I115:I120"/>
+    <mergeCell ref="J115:J120"/>
+    <mergeCell ref="A122:A127"/>
+    <mergeCell ref="B122:B127"/>
+    <mergeCell ref="C122:C127"/>
+    <mergeCell ref="E122:E127"/>
+    <mergeCell ref="F122:F127"/>
+    <mergeCell ref="H122:H127"/>
+    <mergeCell ref="I122:I127"/>
+    <mergeCell ref="J122:J127"/>
+    <mergeCell ref="C115:C120"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="E115:E120"/>
+    <mergeCell ref="F115:F120"/>
+    <mergeCell ref="H115:H120"/>
+    <mergeCell ref="H102:H106"/>
+    <mergeCell ref="I102:I106"/>
+    <mergeCell ref="J102:J106"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="C108:C112"/>
+    <mergeCell ref="E108:E112"/>
+    <mergeCell ref="F108:F112"/>
+    <mergeCell ref="H108:H112"/>
+    <mergeCell ref="I108:I112"/>
+    <mergeCell ref="J108:J112"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="C102:C106"/>
+    <mergeCell ref="E102:E106"/>
+    <mergeCell ref="F102:F106"/>
+    <mergeCell ref="H89:H93"/>
+    <mergeCell ref="I89:I93"/>
+    <mergeCell ref="J89:J93"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="C96:C100"/>
+    <mergeCell ref="E96:E100"/>
+    <mergeCell ref="F96:F100"/>
+    <mergeCell ref="H95:H99"/>
+    <mergeCell ref="I95:I99"/>
+    <mergeCell ref="J95:J99"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="E89:E93"/>
+    <mergeCell ref="F89:F93"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="F82:F86"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="I76:I80"/>
+    <mergeCell ref="J76:J80"/>
+    <mergeCell ref="H82:H86"/>
+    <mergeCell ref="I82:I86"/>
+    <mergeCell ref="J82:J86"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="H62:H67"/>
+    <mergeCell ref="I62:I67"/>
+    <mergeCell ref="J62:J67"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="E69:E74"/>
+    <mergeCell ref="F69:F74"/>
+    <mergeCell ref="H69:H74"/>
+    <mergeCell ref="I69:I74"/>
+    <mergeCell ref="J69:J74"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="E62:E67"/>
+    <mergeCell ref="F62:F67"/>
+    <mergeCell ref="H48:H53"/>
+    <mergeCell ref="I48:I53"/>
+    <mergeCell ref="J48:J53"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="E55:E60"/>
+    <mergeCell ref="F55:F60"/>
+    <mergeCell ref="H55:H60"/>
+    <mergeCell ref="I55:I60"/>
+    <mergeCell ref="J55:J60"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="E48:E53"/>
+    <mergeCell ref="F48:F53"/>
+    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="F41:F46"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="H34:H38"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="H171:H176"/>
+    <mergeCell ref="I171:I176"/>
+    <mergeCell ref="J171:J176"/>
+    <mergeCell ref="A179:A184"/>
+    <mergeCell ref="B179:B184"/>
+    <mergeCell ref="C179:C184"/>
+    <mergeCell ref="E179:E183"/>
+    <mergeCell ref="F179:F183"/>
+    <mergeCell ref="H179:H184"/>
+    <mergeCell ref="I179:I184"/>
+    <mergeCell ref="J179:J184"/>
+    <mergeCell ref="C171:C176"/>
+    <mergeCell ref="J186:J191"/>
+    <mergeCell ref="H186:H191"/>
+    <mergeCell ref="I186:I191"/>
+    <mergeCell ref="A193:A198"/>
+    <mergeCell ref="B193:B198"/>
+    <mergeCell ref="C193:C198"/>
+    <mergeCell ref="E193:E197"/>
+    <mergeCell ref="F193:F197"/>
+    <mergeCell ref="H193:H198"/>
+    <mergeCell ref="I193:I198"/>
+    <mergeCell ref="J193:J198"/>
+    <mergeCell ref="A186:A191"/>
+    <mergeCell ref="B186:B191"/>
+    <mergeCell ref="C186:C191"/>
+    <mergeCell ref="E186:E190"/>
+    <mergeCell ref="F186:F190"/>
+    <mergeCell ref="A200:A205"/>
+    <mergeCell ref="B200:B205"/>
+    <mergeCell ref="C200:C205"/>
+    <mergeCell ref="E200:E204"/>
+    <mergeCell ref="F200:F204"/>
+    <mergeCell ref="H200:H205"/>
+    <mergeCell ref="I200:I205"/>
+    <mergeCell ref="J200:J205"/>
+    <mergeCell ref="A207:A212"/>
+    <mergeCell ref="B207:B212"/>
+    <mergeCell ref="C207:C212"/>
+    <mergeCell ref="H207:H212"/>
+    <mergeCell ref="I207:I212"/>
+    <mergeCell ref="J207:J212"/>
+    <mergeCell ref="F207:F212"/>
+    <mergeCell ref="E207:E212"/>
+    <mergeCell ref="A214:A219"/>
+    <mergeCell ref="B214:B219"/>
+    <mergeCell ref="C214:C219"/>
+    <mergeCell ref="E214:E219"/>
+    <mergeCell ref="F214:F219"/>
+    <mergeCell ref="H214:H219"/>
+    <mergeCell ref="I214:I219"/>
+    <mergeCell ref="J214:J219"/>
+    <mergeCell ref="A221:A226"/>
+    <mergeCell ref="B221:B226"/>
+    <mergeCell ref="C221:C226"/>
+    <mergeCell ref="E221:E226"/>
+    <mergeCell ref="F221:F226"/>
+    <mergeCell ref="H221:H226"/>
+    <mergeCell ref="I221:I226"/>
+    <mergeCell ref="J221:J226"/>
     <mergeCell ref="I235:I240"/>
     <mergeCell ref="J235:J240"/>
     <mergeCell ref="H228:H233"/>
@@ -5699,266 +5927,38 @@
     <mergeCell ref="B235:B240"/>
     <mergeCell ref="C235:C240"/>
     <mergeCell ref="H235:H240"/>
-    <mergeCell ref="A214:A219"/>
-    <mergeCell ref="B214:B219"/>
-    <mergeCell ref="C214:C219"/>
-    <mergeCell ref="E214:E219"/>
-    <mergeCell ref="F214:F219"/>
-    <mergeCell ref="H214:H219"/>
-    <mergeCell ref="I214:I219"/>
-    <mergeCell ref="J214:J219"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="B221:B226"/>
-    <mergeCell ref="C221:C226"/>
-    <mergeCell ref="E221:E226"/>
-    <mergeCell ref="F221:F226"/>
-    <mergeCell ref="H221:H226"/>
-    <mergeCell ref="I221:I226"/>
-    <mergeCell ref="J221:J226"/>
-    <mergeCell ref="A200:A205"/>
-    <mergeCell ref="B200:B205"/>
-    <mergeCell ref="C200:C205"/>
-    <mergeCell ref="E200:E204"/>
-    <mergeCell ref="F200:F204"/>
-    <mergeCell ref="H200:H205"/>
-    <mergeCell ref="I200:I205"/>
-    <mergeCell ref="J200:J205"/>
-    <mergeCell ref="A207:A212"/>
-    <mergeCell ref="B207:B212"/>
-    <mergeCell ref="C207:C212"/>
-    <mergeCell ref="H207:H212"/>
-    <mergeCell ref="I207:I212"/>
-    <mergeCell ref="J207:J212"/>
-    <mergeCell ref="F207:F212"/>
-    <mergeCell ref="E207:E212"/>
-    <mergeCell ref="J186:J191"/>
-    <mergeCell ref="H186:H191"/>
-    <mergeCell ref="I186:I191"/>
-    <mergeCell ref="A193:A198"/>
-    <mergeCell ref="B193:B198"/>
-    <mergeCell ref="C193:C198"/>
-    <mergeCell ref="E193:E197"/>
-    <mergeCell ref="F193:F197"/>
-    <mergeCell ref="H193:H198"/>
-    <mergeCell ref="I193:I198"/>
-    <mergeCell ref="J193:J198"/>
-    <mergeCell ref="A186:A191"/>
-    <mergeCell ref="B186:B191"/>
-    <mergeCell ref="C186:C191"/>
-    <mergeCell ref="E186:E190"/>
-    <mergeCell ref="F186:F190"/>
-    <mergeCell ref="H171:H176"/>
-    <mergeCell ref="I171:I176"/>
-    <mergeCell ref="J171:J176"/>
-    <mergeCell ref="A179:A184"/>
-    <mergeCell ref="B179:B184"/>
-    <mergeCell ref="C179:C184"/>
-    <mergeCell ref="E179:E183"/>
-    <mergeCell ref="F179:F183"/>
-    <mergeCell ref="H179:H184"/>
-    <mergeCell ref="I179:I184"/>
-    <mergeCell ref="J179:J184"/>
-    <mergeCell ref="J20:J24"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="I14:I17"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="J27:J31"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="F41:F46"/>
-    <mergeCell ref="H41:H45"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="H34:H38"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="J34:J38"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="H48:H53"/>
-    <mergeCell ref="I48:I53"/>
-    <mergeCell ref="J48:J53"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="C55:C60"/>
-    <mergeCell ref="E55:E60"/>
-    <mergeCell ref="F55:F60"/>
-    <mergeCell ref="H55:H60"/>
-    <mergeCell ref="I55:I60"/>
-    <mergeCell ref="J55:J60"/>
-    <mergeCell ref="A48:A53"/>
-    <mergeCell ref="B48:B53"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="E48:E53"/>
-    <mergeCell ref="F48:F53"/>
-    <mergeCell ref="H62:H67"/>
-    <mergeCell ref="I62:I67"/>
-    <mergeCell ref="J62:J67"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="B69:B74"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="E69:E74"/>
-    <mergeCell ref="F69:F74"/>
-    <mergeCell ref="H69:H74"/>
-    <mergeCell ref="I69:I74"/>
-    <mergeCell ref="J69:J74"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="E62:E67"/>
-    <mergeCell ref="F62:F67"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="F82:F86"/>
-    <mergeCell ref="H76:H80"/>
-    <mergeCell ref="I76:I80"/>
-    <mergeCell ref="J76:J80"/>
-    <mergeCell ref="H82:H86"/>
-    <mergeCell ref="I82:I86"/>
-    <mergeCell ref="J82:J86"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="E76:E80"/>
-    <mergeCell ref="F76:F80"/>
-    <mergeCell ref="H89:H93"/>
-    <mergeCell ref="I89:I93"/>
-    <mergeCell ref="J89:J93"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="C96:C100"/>
-    <mergeCell ref="E96:E100"/>
-    <mergeCell ref="F96:F100"/>
-    <mergeCell ref="H95:H99"/>
-    <mergeCell ref="I95:I99"/>
-    <mergeCell ref="J95:J99"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="C89:C93"/>
-    <mergeCell ref="E89:E93"/>
-    <mergeCell ref="F89:F93"/>
-    <mergeCell ref="H102:H106"/>
-    <mergeCell ref="I102:I106"/>
-    <mergeCell ref="J102:J106"/>
-    <mergeCell ref="A108:A112"/>
-    <mergeCell ref="B108:B112"/>
-    <mergeCell ref="C108:C112"/>
-    <mergeCell ref="E108:E112"/>
-    <mergeCell ref="F108:F112"/>
-    <mergeCell ref="H108:H112"/>
-    <mergeCell ref="I108:I112"/>
-    <mergeCell ref="J108:J112"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="B102:B106"/>
-    <mergeCell ref="C102:C106"/>
-    <mergeCell ref="E102:E106"/>
-    <mergeCell ref="F102:F106"/>
-    <mergeCell ref="I115:I120"/>
-    <mergeCell ref="J115:J120"/>
-    <mergeCell ref="A122:A127"/>
-    <mergeCell ref="B122:B127"/>
-    <mergeCell ref="C122:C127"/>
-    <mergeCell ref="E122:E127"/>
-    <mergeCell ref="F122:F127"/>
-    <mergeCell ref="H122:H127"/>
-    <mergeCell ref="I122:I127"/>
-    <mergeCell ref="J122:J127"/>
-    <mergeCell ref="C115:C120"/>
-    <mergeCell ref="B115:B120"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="E115:E120"/>
-    <mergeCell ref="F115:F120"/>
-    <mergeCell ref="H115:H120"/>
-    <mergeCell ref="J129:J134"/>
-    <mergeCell ref="A136:A141"/>
-    <mergeCell ref="B136:B141"/>
-    <mergeCell ref="C136:C141"/>
-    <mergeCell ref="E136:E141"/>
-    <mergeCell ref="F136:F141"/>
-    <mergeCell ref="H136:H141"/>
-    <mergeCell ref="I136:I141"/>
-    <mergeCell ref="J136:J141"/>
-    <mergeCell ref="A129:A134"/>
-    <mergeCell ref="B129:B134"/>
-    <mergeCell ref="C129:C134"/>
-    <mergeCell ref="E129:E134"/>
-    <mergeCell ref="F129:F134"/>
-    <mergeCell ref="H129:H134"/>
-    <mergeCell ref="I129:I134"/>
-    <mergeCell ref="H143:H148"/>
-    <mergeCell ref="I143:I148"/>
-    <mergeCell ref="J143:J148"/>
-    <mergeCell ref="A150:A155"/>
-    <mergeCell ref="B150:B155"/>
-    <mergeCell ref="C150:C155"/>
-    <mergeCell ref="E150:E154"/>
-    <mergeCell ref="F150:F154"/>
-    <mergeCell ref="H150:H155"/>
-    <mergeCell ref="I150:I155"/>
-    <mergeCell ref="J150:J155"/>
-    <mergeCell ref="C171:C176"/>
-    <mergeCell ref="E157:E161"/>
-    <mergeCell ref="F157:F161"/>
-    <mergeCell ref="B164:B169"/>
-    <mergeCell ref="B171:B176"/>
-    <mergeCell ref="A164:A169"/>
-    <mergeCell ref="A171:A176"/>
-    <mergeCell ref="A143:A148"/>
-    <mergeCell ref="B143:B148"/>
-    <mergeCell ref="C143:C148"/>
-    <mergeCell ref="E143:E148"/>
-    <mergeCell ref="F143:F148"/>
-    <mergeCell ref="E171:E175"/>
-    <mergeCell ref="F171:F175"/>
-    <mergeCell ref="H157:H162"/>
-    <mergeCell ref="I157:I162"/>
-    <mergeCell ref="J157:J162"/>
-    <mergeCell ref="H164:H169"/>
-    <mergeCell ref="I164:I169"/>
-    <mergeCell ref="J164:J169"/>
-    <mergeCell ref="E164:E168"/>
-    <mergeCell ref="F164:F168"/>
-    <mergeCell ref="A157:A162"/>
-    <mergeCell ref="B157:B162"/>
-    <mergeCell ref="C157:C162"/>
-    <mergeCell ref="C164:C169"/>
+    <mergeCell ref="B249:B254"/>
+    <mergeCell ref="A249:A254"/>
+    <mergeCell ref="C249:C254"/>
+    <mergeCell ref="E249:E254"/>
+    <mergeCell ref="F249:F254"/>
+    <mergeCell ref="H249:H254"/>
+    <mergeCell ref="I249:I254"/>
+    <mergeCell ref="J249:J254"/>
+    <mergeCell ref="A256:A261"/>
+    <mergeCell ref="B256:B261"/>
+    <mergeCell ref="C256:C261"/>
+    <mergeCell ref="E256:E261"/>
+    <mergeCell ref="F256:F261"/>
+    <mergeCell ref="H256:H261"/>
+    <mergeCell ref="I256:I261"/>
+    <mergeCell ref="J256:J261"/>
+    <mergeCell ref="H263:H268"/>
+    <mergeCell ref="I263:I268"/>
+    <mergeCell ref="J263:J268"/>
+    <mergeCell ref="H270:H275"/>
+    <mergeCell ref="I270:I275"/>
+    <mergeCell ref="J270:J275"/>
+    <mergeCell ref="A263:A268"/>
+    <mergeCell ref="B263:B268"/>
+    <mergeCell ref="C263:C268"/>
+    <mergeCell ref="A270:A275"/>
+    <mergeCell ref="B270:B275"/>
+    <mergeCell ref="C270:C275"/>
+    <mergeCell ref="E263:E267"/>
+    <mergeCell ref="E270:E274"/>
+    <mergeCell ref="F270:F274"/>
+    <mergeCell ref="F263:F267"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>